<commit_message>
Couple updates to Rshiny converter used to send energy farm data to Rojda
</commit_message>
<xml_diff>
--- a/Fluxes_varnames_rshiny.xlsx
+++ b/Fluxes_varnames_rshiny.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" calcOnSave="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="69">
   <si>
     <t>DateTime</t>
   </si>
@@ -179,15 +179,9 @@
     <t>Fh</t>
   </si>
   <si>
-    <t>Fh_EPFlag</t>
-  </si>
-  <si>
     <t>Fe</t>
   </si>
   <si>
-    <t>Fe_EPFlag</t>
-  </si>
-  <si>
     <t>RH</t>
   </si>
   <si>
@@ -209,9 +203,6 @@
     <t>Fco2</t>
   </si>
   <si>
-    <t>Fco2_EPFlag</t>
-  </si>
-  <si>
     <t>ps</t>
   </si>
   <si>
@@ -222,6 +213,24 @@
   </si>
   <si>
     <t>VPD</t>
+  </si>
+  <si>
+    <t>Older: Fh_EPFlag</t>
+  </si>
+  <si>
+    <t>Older: Fco2_EPFlag</t>
+  </si>
+  <si>
+    <t>Fco2_EP_QC</t>
+  </si>
+  <si>
+    <t>Fh_EP_QC</t>
+  </si>
+  <si>
+    <t>Older: Fe_EPFlag</t>
+  </si>
+  <si>
+    <t>Fe_EP_QC</t>
   </si>
 </sst>
 </file>
@@ -549,10 +558,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T7"/>
+  <dimension ref="A1:T9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P17" sqref="P17"/>
+      <selection activeCell="P11" sqref="P11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -762,49 +771,49 @@
         <v>49</v>
       </c>
       <c r="B5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C5" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="D5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E5" t="s">
         <v>50</v>
       </c>
       <c r="F5" t="s">
+        <v>66</v>
+      </c>
+      <c r="G5" t="s">
         <v>51</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I5" t="s">
+        <v>59</v>
+      </c>
+      <c r="J5" t="s">
+        <v>56</v>
+      </c>
+      <c r="L5" t="s">
         <v>52</v>
       </c>
-      <c r="H5" t="s">
+      <c r="M5" t="s">
         <v>53</v>
       </c>
-      <c r="I5" t="s">
+      <c r="N5" t="s">
+        <v>54</v>
+      </c>
+      <c r="P5" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>61</v>
+      </c>
+      <c r="S5" t="s">
         <v>62</v>
-      </c>
-      <c r="J5" t="s">
-        <v>58</v>
-      </c>
-      <c r="L5" t="s">
-        <v>54</v>
-      </c>
-      <c r="M5" t="s">
-        <v>55</v>
-      </c>
-      <c r="N5" t="s">
-        <v>56</v>
-      </c>
-      <c r="P5" t="s">
-        <v>63</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>64</v>
-      </c>
-      <c r="S5" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
@@ -839,7 +848,7 @@
         <v>0.67130000000000001</v>
       </c>
       <c r="K6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="M6" s="1">
         <v>-9999</v>
@@ -848,7 +857,7 @@
         <v>-9999</v>
       </c>
       <c r="O6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="P6">
         <v>272.47119529999998</v>
@@ -857,10 +866,10 @@
         <v>280.43016666666665</v>
       </c>
       <c r="R6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="T6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
@@ -895,7 +904,7 @@
         <v>1.02</v>
       </c>
       <c r="K7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="L7">
         <v>90.603800000000007</v>
@@ -907,7 +916,7 @@
         <v>0.24099999999999999</v>
       </c>
       <c r="O7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="P7">
         <v>272.46355449999999</v>
@@ -916,13 +925,24 @@
         <v>278.04199999999997</v>
       </c>
       <c r="R7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="S7">
         <v>53.0657</v>
       </c>
       <c r="T7" t="s">
-        <v>57</v>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>64</v>
+      </c>
+      <c r="F9" t="s">
+        <v>63</v>
+      </c>
+      <c r="H9" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>